<commit_message>
Working time update + Scripts
</commit_message>
<xml_diff>
--- a/doc/synch-db-working-hours-janeczek-mair.xlsx
+++ b/doc/synch-db-working-hours-janeczek-mair.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Desktop\git\synch-db\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Janeczek" sheetId="8" r:id="rId1"/>
@@ -22,12 +17,12 @@
     <definedName name="SumEstJaneczek">Janeczek!$E$12</definedName>
     <definedName name="SumEstMair">Mair!$E$10</definedName>
   </definedNames>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t>PHASE</t>
   </si>
@@ -72,16 +67,22 @@
   </si>
   <si>
     <t>ER-Diagram in Astah</t>
+  </si>
+  <si>
+    <t>Programming</t>
+  </si>
+  <si>
+    <t>Create-Script + Inserts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -266,9 +267,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Gut" xfId="1" builtinId="26"/>
+    <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -352,9 +353,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -392,9 +393,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -426,10 +427,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -461,10 +461,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -637,24 +636,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" style="13" customWidth="1"/>
-    <col min="4" max="4" width="35.44140625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" style="13" customWidth="1"/>
     <col min="5" max="5" width="12" style="13" customWidth="1"/>
     <col min="6" max="6" width="9" style="13" customWidth="1"/>
-    <col min="7" max="7" width="59.33203125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="59.28515625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -662,7 +661,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="25" t="s">
         <v>10</v>
@@ -673,7 +672,7 @@
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -681,7 +680,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:7" s="13" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="13" customFormat="1" ht="15.6" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="4" t="s">
         <v>6</v>
@@ -702,7 +701,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15.6" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="5">
         <v>41936</v>
@@ -723,7 +722,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15.6" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="5"/>
       <c r="C6" s="15"/>
@@ -732,7 +731,7 @@
       <c r="F6" s="20"/>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15.6" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="5"/>
       <c r="C7" s="15"/>
@@ -741,7 +740,7 @@
       <c r="F7" s="20"/>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:7" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="29.45" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="5"/>
       <c r="C8" s="15"/>
@@ -750,7 +749,7 @@
       <c r="F8" s="19"/>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15.6" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="5"/>
       <c r="C9" s="15"/>
@@ -759,7 +758,7 @@
       <c r="F9" s="20"/>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="31.9" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="5"/>
       <c r="C10" s="15"/>
@@ -768,7 +767,7 @@
       <c r="F10" s="20"/>
       <c r="G10" s="11"/>
     </row>
-    <row r="11" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15.6" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="5"/>
       <c r="C11" s="15"/>
@@ -777,7 +776,7 @@
       <c r="F11" s="16"/>
       <c r="G11" s="11"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="A12" s="1"/>
       <c r="B12" s="24" t="s">
         <v>7</v>
@@ -794,7 +793,7 @@
       </c>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
@@ -802,7 +801,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
@@ -810,7 +809,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
@@ -818,7 +817,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
@@ -837,23 +836,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.109375"/>
-    <col min="3" max="3" width="15.5546875" style="13" customWidth="1"/>
-    <col min="4" max="4" width="37.6640625" style="13"/>
-    <col min="5" max="5" width="14.88671875" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" style="13"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -861,7 +861,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="25" t="s">
         <v>10</v>
@@ -872,7 +872,7 @@
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -880,7 +880,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15.6" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="4" t="s">
         <v>6</v>
@@ -901,7 +901,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5" s="1"/>
       <c r="B5" s="5">
         <v>41936</v>
@@ -922,16 +922,26 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6" s="1"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="19"/>
+      <c r="B6" s="5">
+        <v>41956</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="19">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F6" s="20">
+        <v>2.7777777777777776E-2</v>
+      </c>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7" s="1"/>
       <c r="B7" s="5"/>
       <c r="C7" s="15"/>
@@ -940,7 +950,7 @@
       <c r="F7" s="19"/>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8" s="1"/>
       <c r="B8" s="5"/>
       <c r="C8" s="15"/>
@@ -949,7 +959,7 @@
       <c r="F8" s="20"/>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9" s="1"/>
       <c r="B9" s="5"/>
       <c r="C9" s="15"/>
@@ -958,7 +968,7 @@
       <c r="F9" s="20"/>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10" s="1"/>
       <c r="B10" s="24" t="s">
         <v>7</v>
@@ -967,15 +977,15 @@
       <c r="D10" s="24"/>
       <c r="E10" s="17">
         <f>SUM(E5:E9)</f>
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="F10" s="17">
         <f>SUM(F5:F9)</f>
-        <v>1.892361111111111E-2</v>
+        <v>4.670138888888889E-2</v>
       </c>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
@@ -983,7 +993,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
@@ -991,7 +1001,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
@@ -999,7 +1009,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
@@ -1018,20 +1028,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:D8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.5546875"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="18.75">
       <c r="A3" s="25" t="s">
         <v>10</v>
       </c>
@@ -1039,11 +1049,11 @@
       <c r="C3" s="25"/>
       <c r="D3" s="25"/>
     </row>
-    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="18.75">
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="B5" s="8" t="s">
         <v>1</v>
       </c>
@@ -1054,7 +1064,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="B6" s="14" t="s">
         <v>2</v>
       </c>
@@ -1067,30 +1077,30 @@
         <v>1.892361111111111E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="B7" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="21">
         <f>SumEstMair</f>
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D7" s="22">
         <f>SumActMair</f>
-        <v>1.892361111111111E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4.670138888888889E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="B8" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="21">
         <f>SUM(SumEstJaneczek+SumEstMair)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
       <c r="D8" s="22">
         <f>SUM(SumActJaneczek+SumActMair)</f>
-        <v>3.784722222222222E-2</v>
+        <v>6.5625000000000003E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CREATE scripts and working hours adjusted
</commit_message>
<xml_diff>
--- a/doc/synch-db-working-hours-janeczek-mair.xlsx
+++ b/doc/synch-db-working-hours-janeczek-mair.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Desktop\git\synch-db\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196"/>
   </bookViews>
   <sheets>
     <sheet name="Janeczek" sheetId="8" r:id="rId1"/>
@@ -17,12 +22,12 @@
     <definedName name="SumEstJaneczek">Janeczek!$E$12</definedName>
     <definedName name="SumEstMair">Mair!$E$10</definedName>
   </definedNames>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>PHASE</t>
   </si>
@@ -73,16 +78,22 @@
   </si>
   <si>
     <t>Create-Script + Inserts</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Technology Description + Further Approach</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -267,9 +278,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Gut" xfId="1" builtinId="26"/>
-    <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -353,9 +364,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -393,9 +404,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -427,9 +438,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -461,9 +473,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -636,24 +649,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" style="13" customWidth="1"/>
     <col min="5" max="5" width="12" style="13" customWidth="1"/>
     <col min="6" max="6" width="9" style="13" customWidth="1"/>
-    <col min="7" max="7" width="59.28515625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="59.33203125" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -661,7 +674,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="25" t="s">
         <v>10</v>
@@ -672,7 +685,7 @@
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -680,7 +693,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:7" s="13" customFormat="1" ht="15.6" customHeight="1">
+    <row r="4" spans="1:7" s="13" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="4" t="s">
         <v>6</v>
@@ -701,7 +714,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.6" customHeight="1">
+    <row r="5" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="5">
         <v>41936</v>
@@ -722,16 +735,26 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.6" customHeight="1">
+    <row r="6" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="20"/>
+      <c r="B6" s="5">
+        <v>41956</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="19">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F6" s="20">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:7" ht="15.6" customHeight="1">
+    <row r="7" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="5"/>
       <c r="C7" s="15"/>
@@ -740,7 +763,7 @@
       <c r="F7" s="20"/>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:7" ht="29.45" customHeight="1">
+    <row r="8" spans="1:7" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="5"/>
       <c r="C8" s="15"/>
@@ -749,7 +772,7 @@
       <c r="F8" s="19"/>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:7" ht="15.6" customHeight="1">
+    <row r="9" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="5"/>
       <c r="C9" s="15"/>
@@ -758,7 +781,7 @@
       <c r="F9" s="20"/>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:7" ht="31.9" customHeight="1">
+    <row r="10" spans="1:7" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="5"/>
       <c r="C10" s="15"/>
@@ -767,7 +790,7 @@
       <c r="F10" s="20"/>
       <c r="G10" s="11"/>
     </row>
-    <row r="11" spans="1:7" ht="15.6" customHeight="1">
+    <row r="11" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="5"/>
       <c r="C11" s="15"/>
@@ -776,7 +799,7 @@
       <c r="F11" s="16"/>
       <c r="G11" s="11"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="24" t="s">
         <v>7</v>
@@ -785,15 +808,15 @@
       <c r="D12" s="24"/>
       <c r="E12" s="17">
         <f>SUM(E5:E11)</f>
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="F12" s="17">
         <f>SUM(F5:F11)</f>
-        <v>1.892361111111111E-2</v>
+        <v>3.9756944444444442E-2</v>
       </c>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
@@ -801,7 +824,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
@@ -809,7 +832,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
@@ -817,7 +840,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
@@ -836,24 +859,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="37.7109375" style="13"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="37.6640625" style="13"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -861,7 +884,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="25" t="s">
         <v>10</v>
@@ -872,7 +895,7 @@
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -880,7 +903,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="15.6" customHeight="1">
+    <row r="4" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="4" t="s">
         <v>6</v>
@@ -901,7 +924,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="5">
         <v>41936</v>
@@ -922,7 +945,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="5">
         <v>41956</v>
@@ -941,7 +964,7 @@
       </c>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="5"/>
       <c r="C7" s="15"/>
@@ -950,7 +973,7 @@
       <c r="F7" s="19"/>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="5"/>
       <c r="C8" s="15"/>
@@ -959,7 +982,7 @@
       <c r="F8" s="20"/>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="5"/>
       <c r="C9" s="15"/>
@@ -968,7 +991,7 @@
       <c r="F9" s="20"/>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="24" t="s">
         <v>7</v>
@@ -985,7 +1008,7 @@
       </c>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
@@ -993,7 +1016,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
@@ -1001,7 +1024,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
@@ -1009,7 +1032,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
@@ -1028,20 +1051,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.5703125"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" ht="18.75">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>10</v>
       </c>
@@ -1049,11 +1072,11 @@
       <c r="C3" s="25"/>
       <c r="D3" s="25"/>
     </row>
-    <row r="4" spans="1:4" ht="18.75">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>1</v>
       </c>
@@ -1064,20 +1087,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="21">
         <f>SumEstJaneczek</f>
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D6" s="22">
         <f>SumActJaneczek</f>
-        <v>1.892361111111111E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>3.9756944444444442E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" s="14" t="s">
         <v>3</v>
       </c>
@@ -1090,17 +1113,17 @@
         <v>4.670138888888889E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="21">
         <f>SUM(SumEstJaneczek+SumEstMair)</f>
-        <v>0.125</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D8" s="22">
         <f>SUM(SumActJaneczek+SumActMair)</f>
-        <v>6.5625000000000003E-2</v>
+        <v>8.6458333333333331E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>